<commit_message>
Looking at Alt 1 solution
</commit_message>
<xml_diff>
--- a/Excel_Challenge_498 - Soccer Champions Alignment.xlsx
+++ b/Excel_Challenge_498 - Soccer Champions Alignment.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AE0088-89A0-49A1-8052-A21485D61A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0882D-26F8-4C97-89E0-5E91595578AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F54B996A-C2D2-412A-8E54-11CA84F94FE3}"/>
+    <workbookView xWindow="-18750" yWindow="230" windowWidth="18870" windowHeight="20330" activeTab="3" xr2:uid="{F54B996A-C2D2-412A-8E54-11CA84F94FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="2" r:id="rId1"/>
     <sheet name="EDA" sheetId="3" r:id="rId2"/>
     <sheet name="MySingleFunction" sheetId="4" r:id="rId3"/>
+    <sheet name="Alt" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Alt!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!#REF!</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="22">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -129,12 +131,15 @@
   <si>
     <t>1950, 1930</t>
   </si>
+  <si>
+    <t>Link</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +151,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,15 +193,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -692,6 +708,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -703,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F52D858-0BD2-467F-84F0-576111609A89}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,13 +737,13 @@
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -737,8 +756,11 @@
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -752,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -766,7 +788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -780,7 +802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -794,7 +816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -808,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -822,7 +844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -836,7 +858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -850,7 +872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>1990</v>
       </c>
@@ -858,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D12">
         <v>1986</v>
       </c>
@@ -866,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D13">
         <v>1982</v>
       </c>
@@ -874,7 +896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14">
         <v>1978</v>
       </c>
@@ -882,7 +904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>1974</v>
       </c>
@@ -890,7 +912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>1970</v>
       </c>
@@ -963,9 +985,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{69BDA466-43A8-41A2-B15D-67600D13FC49}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1734,7 +1759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169323CA-045F-470F-8E38-B08A45D52C2A}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2146,4 +2171,466 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C790FA-F128-46E7-B37E-F152F4ECCEE6}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.109375" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>2022</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>2014</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2010</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>2006</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2002</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>1998</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>1994</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1990</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1986</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>1982</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>1978</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>1974</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>1970</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>1966</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>1962</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1958</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>1954</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>1950</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1938</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>1934</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>1930</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="str" cm="1">
+        <f t="array" ref="B28:C50">_xlfn.LET(_xlpm.y, -MID(B3:B10, _xlfn.SEQUENCE(, 5, ,6), 4), _xlfn.VSTACK(D2:E2, _xlfn._xlws.SORT(MID(_xlfn.TOCOL(-_xlpm.y&amp;A3:A10, 2), {1,5}, {4,9}), , -1)))</f>
+        <v>Year</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Winner</v>
+      </c>
+      <c r="F28" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B28)</f>
+        <v>=LET(y, -MID(B3:B10, SEQUENCE(, 5, ,6), 4), VSTACK(D2:E2, SORT(MID(TOCOL(-y&amp;A3:A10, 2), {1,5}, {4,9}), , -1)))</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <v>2022</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <v>2018</v>
+      </c>
+      <c r="C30" t="str">
+        <v>France</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <v>2014</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <v>2010</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Spain</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <v>2006</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="str">
+        <v>2002</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="str">
+        <v>1998</v>
+      </c>
+      <c r="C35" t="str">
+        <v>France</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="str">
+        <v>1994</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="str">
+        <v>1990</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="str">
+        <v>1986</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="str">
+        <v>1982</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="str">
+        <v>1978</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="str">
+        <v>1974</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="str">
+        <v>1970</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" t="str">
+        <v>1966</v>
+      </c>
+      <c r="C43" t="str">
+        <v>England</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" t="str">
+        <v>1962</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" t="str">
+        <v>1958</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="str">
+        <v>1954</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="str">
+        <v>1950</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Uruguay</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="str">
+        <v>1938</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="str">
+        <v>1934</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="str">
+        <v>1930</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Uruguay</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{FDE85C45-E2D4-4E01-B0B9-FFA0000D268B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Looking at Alt 2, great use of EXPAND function
</commit_message>
<xml_diff>
--- a/Excel_Challenge_498 - Soccer Champions Alignment.xlsx
+++ b/Excel_Challenge_498 - Soccer Champions Alignment.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0882D-26F8-4C97-89E0-5E91595578AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A871008-490F-41AF-AB17-12B6F65A300A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18750" yWindow="230" windowWidth="18870" windowHeight="20330" activeTab="3" xr2:uid="{F54B996A-C2D2-412A-8E54-11CA84F94FE3}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{F54B996A-C2D2-412A-8E54-11CA84F94FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="2" r:id="rId1"/>
     <sheet name="EDA" sheetId="3" r:id="rId2"/>
     <sheet name="MySingleFunction" sheetId="4" r:id="rId3"/>
     <sheet name="Alt" sheetId="5" r:id="rId4"/>
+    <sheet name="Alt2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Alt!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt2'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!#REF!</definedName>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="24">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -134,12 +136,18 @@
   <si>
     <t>Link</t>
   </si>
+  <si>
+    <t>Uses offset, makes it volatile.</t>
+  </si>
+  <si>
+    <t>This solution has the best use of Expand that I have seen yet. Basically, this guy uses it as a substitute for filldown.Great use.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +167,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,11 +212,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -692,7 +708,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="864" row="9">
+  <wetp:taskpane dockstate="right" visibility="0" width="1187" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2177,7 +2193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C790FA-F128-46E7-B37E-F152F4ECCEE6}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -2633,4 +2649,545 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D36D01E-34F7-4F95-BFB0-E0ABCB02CE0C}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.109375" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>2022</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>2014</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2010</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>2006</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2002</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>1998</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>1994</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1990</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1986</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>1982</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>1978</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>1974</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>1970</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>1966</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>1962</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1958</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>1954</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>1950</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1938</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>1934</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>1930</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="str" cm="1">
+        <f t="array" aca="1" ref="B28:C50" ca="1">_xlfn._xlws.SORT(
+    _xlfn.REDUCE(
+        {"Year","Winner"},
+        A3:A10,
+        _xlfn.LAMBDA(_xlpm.x,_xlpm.y,
+            _xlfn.LET(
+                _xlpm.a, _xlfn.TEXTSPLIT(OFFSET(_xlpm.y, , 1), , ", "),
+                _xlfn.VSTACK(_xlpm.x, _xlfn.HSTACK(_xlpm.a, _xlfn.EXPAND(_xlpm.y, COUNTA(_xlpm.a), , _xlpm.y)))
+            )
+        )
+    ),
+    ,
+    -1
+)</f>
+        <v>Year</v>
+      </c>
+      <c r="C28" t="str">
+        <f ca="1"/>
+        <v>Winner</v>
+      </c>
+      <c r="F28" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B28)</f>
+        <v>=SORT(
+    REDUCE(
+        {"Year","Winner"},
+        A3:A10,
+        LAMBDA(x,y,
+            LET(
+                a, TEXTSPLIT(OFFSET(y, , 1), , ", "),
+                VSTACK(x, HSTACK(a, EXPAND(y, COUNTA(a), , y)))
+            )
+        )
+    ),
+    ,
+    -1
+)</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <f ca="1"/>
+        <v>2022</v>
+      </c>
+      <c r="C29" t="str">
+        <f ca="1"/>
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <f ca="1"/>
+        <v>2018</v>
+      </c>
+      <c r="C30" t="str">
+        <f ca="1"/>
+        <v>France</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <f ca="1"/>
+        <v>2014</v>
+      </c>
+      <c r="C31" t="str">
+        <f ca="1"/>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <f ca="1"/>
+        <v>2010</v>
+      </c>
+      <c r="C32" t="str">
+        <f ca="1"/>
+        <v>Spain</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <f ca="1"/>
+        <v>2006</v>
+      </c>
+      <c r="C33" t="str">
+        <f ca="1"/>
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="str">
+        <f ca="1"/>
+        <v>2002</v>
+      </c>
+      <c r="C34" t="str">
+        <f ca="1"/>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="str">
+        <f ca="1"/>
+        <v>1998</v>
+      </c>
+      <c r="C35" t="str">
+        <f ca="1"/>
+        <v>France</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="str">
+        <f ca="1"/>
+        <v>1994</v>
+      </c>
+      <c r="C36" t="str">
+        <f ca="1"/>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="str">
+        <f ca="1"/>
+        <v>1990</v>
+      </c>
+      <c r="C37" t="str">
+        <f ca="1"/>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="str">
+        <f ca="1"/>
+        <v>1986</v>
+      </c>
+      <c r="C38" t="str">
+        <f ca="1"/>
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="str">
+        <f ca="1"/>
+        <v>1982</v>
+      </c>
+      <c r="C39" t="str">
+        <f ca="1"/>
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="str">
+        <f ca="1"/>
+        <v>1978</v>
+      </c>
+      <c r="C40" t="str">
+        <f ca="1"/>
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="str">
+        <f ca="1"/>
+        <v>1974</v>
+      </c>
+      <c r="C41" t="str">
+        <f ca="1"/>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="str">
+        <f ca="1"/>
+        <v>1970</v>
+      </c>
+      <c r="C42" t="str">
+        <f ca="1"/>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" t="str">
+        <f ca="1"/>
+        <v>1966</v>
+      </c>
+      <c r="C43" t="str">
+        <f ca="1"/>
+        <v>England</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" t="str">
+        <f ca="1"/>
+        <v>1962</v>
+      </c>
+      <c r="C44" t="str">
+        <f ca="1"/>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" t="str">
+        <f ca="1"/>
+        <v>1958</v>
+      </c>
+      <c r="C45" t="str">
+        <f ca="1"/>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="str">
+        <f ca="1"/>
+        <v>1954</v>
+      </c>
+      <c r="C46" t="str">
+        <f ca="1"/>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="str">
+        <f ca="1"/>
+        <v>1950</v>
+      </c>
+      <c r="C47" t="str">
+        <f ca="1"/>
+        <v>Uruguay</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="str">
+        <f ca="1"/>
+        <v>1938</v>
+      </c>
+      <c r="C48" t="str">
+        <f ca="1"/>
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="str">
+        <f ca="1"/>
+        <v>1934</v>
+      </c>
+      <c r="C49" t="str">
+        <f ca="1"/>
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="str">
+        <f ca="1"/>
+        <v>1930</v>
+      </c>
+      <c r="C50" t="str">
+        <f ca="1"/>
+        <v>Uruguay</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{5E8C51EC-5BA0-44B3-95DF-58FA7119981B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>